<commit_message>
add multi thread, fix textbox, format code
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,12 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Path</t>
   </si>
   <si>
     <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Users/lanhdang/Projects/mmo/add-text-to-videos/video1.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thuốc thông minh, uống một liều duy nhất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Users/lanhdang/Projects/mmo/add-text-to-videos/video3.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thuốc thử độ ngu, uống càng nhiều càng cho kết quả chính xác</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Users/lanhdang/Projects/mmo/add-text-to-videos/video12.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thuốc làm giàu, uống vào giàu ngay!!!!</t>
   </si>
 </sst>
 </file>
@@ -100,12 +118,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -126,19 +140,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.16"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -146,8 +160,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix path support windows
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -143,10 +143,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:B8"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.16"/>

</xml_diff>